<commit_message>
Finished the art for the Spellcaster searcher, which I've changed the name of to Assistant Magician, and the art source to Boo Koo.
</commit_message>
<xml_diff>
--- a/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
+++ b/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Format - 2005-08 Goat\Typal Battle Searchers\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05DD7F2-A9A5-4D9A-A0B4-56E4D375EBE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E3794E-1C38-4000-98A2-AFC96AA7A9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="177">
   <si>
     <t>Attribute</t>
   </si>
@@ -262,9 +262,6 @@
     <t>Barrel Rock</t>
   </si>
   <si>
-    <t>Phantom Dewan</t>
-  </si>
-  <si>
     <t>LaLa Li-Oon</t>
   </si>
   <si>
@@ -313,9 +310,6 @@
     <t>Kairyu-Kotei</t>
   </si>
   <si>
-    <t>Phantom Sorcerer</t>
-  </si>
-  <si>
     <t>Thundercloud</t>
   </si>
   <si>
@@ -548,16 +542,37 @@
   </si>
   <si>
     <t>Machine Soldier</t>
+  </si>
+  <si>
+    <t>Boo Koo</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>Level 4</t>
+  </si>
+  <si>
+    <t>Assistant Magician</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1001,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1076,10 +1091,10 @@
         <v>45</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F2" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2" t="s">
         <v>28</v>
@@ -1110,10 +1125,10 @@
         <v>45</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F3" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="s">
         <v>31</v>
@@ -1144,7 +1159,7 @@
         <v>45</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F4" s="4">
         <v>4</v>
@@ -1178,7 +1193,7 @@
         <v>45</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F5" s="4">
         <v>4</v>
@@ -1250,7 +1265,7 @@
         <v>45</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F7" s="7">
         <v>3</v>
@@ -1291,7 +1306,7 @@
         <v>45</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F8" s="4">
         <v>4</v>
@@ -1325,10 +1340,10 @@
         <v>45</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" t="s">
         <v>28</v>
@@ -1396,25 +1411,29 @@
       <c r="D11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="F11" s="4">
+      <c r="E11" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F11" s="7">
         <v>4</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4" t="s">
+      <c r="H11" s="7">
+        <v>1500</v>
+      </c>
+      <c r="I11" s="7">
+        <v>1000</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="L11" s="4" t="s">
-        <v>82</v>
+      <c r="L11" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="N11" t="s">
         <v>55</v>
@@ -1434,10 +1453,10 @@
         <v>45</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F12" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12" t="s">
         <v>31</v>
@@ -1468,10 +1487,10 @@
         <v>45</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F13" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G13" t="s">
         <v>29</v>
@@ -1502,10 +1521,10 @@
         <v>45</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F14" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G14" t="s">
         <v>30</v>
@@ -1574,7 +1593,7 @@
         <v>45</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F16" s="4">
         <v>4</v>
@@ -1591,7 +1610,7 @@
         <v>64</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1608,16 +1627,20 @@
         <v>45</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="F17" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G17" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="H17" s="4">
+        <v>450</v>
+      </c>
+      <c r="I17" s="4">
+        <v>750</v>
+      </c>
       <c r="J17" s="4" t="s">
         <v>57</v>
       </c>
@@ -1625,7 +1648,7 @@
         <v>64</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>78</v>
+        <v>172</v>
       </c>
       <c r="N17" t="s">
         <v>60</v>
@@ -1645,7 +1668,7 @@
         <v>45</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F18" s="4">
         <v>3</v>
@@ -1662,7 +1685,7 @@
         <v>64</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -1679,10 +1702,10 @@
         <v>45</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F19" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G19" t="s">
         <v>31</v>
@@ -1696,7 +1719,7 @@
         <v>64</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N19" t="s">
         <v>53</v>
@@ -1716,10 +1739,10 @@
         <v>45</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F20" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G20" t="s">
         <v>32</v>
@@ -1733,7 +1756,7 @@
         <v>64</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -1788,7 +1811,7 @@
         <v>47</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F22" s="4">
         <v>4</v>
@@ -1805,7 +1828,7 @@
         <v>64</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -1860,10 +1883,10 @@
         <v>50</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F24" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G24" t="s">
         <v>33</v>
@@ -1877,7 +1900,7 @@
         <v>64</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -1894,10 +1917,10 @@
         <v>48</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F25" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G25" t="s">
         <v>33</v>
@@ -1911,7 +1934,7 @@
         <v>64</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
@@ -1924,6 +1947,13 @@
         <f>COUNTIF(J:J, "*&lt;= 1500 ATK*")</f>
         <v>12</v>
       </c>
+      <c r="J27" t="s">
+        <v>173</v>
+      </c>
+      <c r="K27">
+        <f>COUNTIF(F2:F25, "=2")</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
@@ -1932,6 +1962,13 @@
       <c r="F28">
         <f>COUNTIF(J:J, "*&lt;= 1500 DEF")</f>
         <v>9</v>
+      </c>
+      <c r="J28" t="s">
+        <v>174</v>
+      </c>
+      <c r="K28">
+        <f>COUNTIF(F2:F25, "=3")</f>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
@@ -1944,10 +1981,17 @@
         <f>COUNTIF(J:J, "*&lt;= 2000 DEF*")</f>
         <v>3</v>
       </c>
+      <c r="J29" t="s">
+        <v>175</v>
+      </c>
+      <c r="K29">
+        <f>COUNTIF(F2:F25, "=4")</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F30">
         <f>COUNTIF(J:J, "*DEF*")</f>
@@ -1955,6 +1999,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G1:G26 G28:G1048576 E29:E30">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"DARK"</formula>
@@ -2015,16 +2060,16 @@
         <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -2041,17 +2086,17 @@
         <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2068,16 +2113,16 @@
         <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2094,17 +2139,17 @@
         <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2121,17 +2166,17 @@
         <v>45</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2148,17 +2193,17 @@
         <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2175,14 +2220,14 @@
         <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2199,16 +2244,16 @@
         <v>45</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -2225,16 +2270,16 @@
         <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -2251,16 +2296,16 @@
         <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -2277,13 +2322,13 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="I11" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -2300,16 +2345,16 @@
         <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2326,13 +2371,13 @@
         <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2349,13 +2394,13 @@
         <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2372,16 +2417,16 @@
         <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -2398,17 +2443,17 @@
         <v>45</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -2425,16 +2470,16 @@
         <v>45</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -2451,16 +2496,16 @@
         <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -2477,17 +2522,17 @@
         <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2504,16 +2549,16 @@
         <v>45</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -2530,16 +2575,16 @@
         <v>45</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M21" s="1"/>
     </row>
@@ -2557,7 +2602,7 @@
         <v>47</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -2574,7 +2619,7 @@
         <v>49</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -2594,7 +2639,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -2611,7 +2656,7 @@
         <v>48</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forgot to note down Assistant Magician's art components and add it to the promo collage. Also outlined the next typal searcher: Legendary Samurai of the Wasteland.
</commit_message>
<xml_diff>
--- a/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
+++ b/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Format - 2005-08 Goat\Typal Battle Searchers\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E3794E-1C38-4000-98A2-AFC96AA7A9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2779EE6-BC4A-4FAE-8E94-7CAF4A7BA091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -277,24 +277,15 @@
     <t>Yormungarde</t>
   </si>
   <si>
-    <t>Beautiful Beast Trainer</t>
-  </si>
-  <si>
     <t>Cyber Archfiend</t>
   </si>
   <si>
-    <t>Thought Archfiend</t>
-  </si>
-  <si>
     <t>Ancient Illusionist</t>
   </si>
   <si>
     <t>Naiad</t>
   </si>
   <si>
-    <t>Mountain Battleguard</t>
-  </si>
-  <si>
     <t>Horned Dolphin</t>
   </si>
   <si>
@@ -313,9 +304,6 @@
     <t>Thundercloud</t>
   </si>
   <si>
-    <t>Elf Battlemistress</t>
-  </si>
-  <si>
     <t>Cyberse Monkey</t>
   </si>
   <si>
@@ -557,6 +545,18 @@
   </si>
   <si>
     <t>Assistant Magician</t>
+  </si>
+  <si>
+    <t>Legendary Samurai of the Wasteland</t>
+  </si>
+  <si>
+    <t>Zanki</t>
+  </si>
+  <si>
+    <t>Mountain Sentry</t>
+  </si>
+  <si>
+    <t>Psychic Fiend</t>
   </si>
 </sst>
 </file>
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1032,7 +1032,7 @@
     <col min="8" max="9" width="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" customWidth="1"/>
     <col min="11" max="11" width="9.77734375" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1091,7 +1091,7 @@
         <v>45</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F2" s="4">
         <v>2</v>
@@ -1125,7 +1125,7 @@
         <v>45</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F3" s="4">
         <v>2</v>
@@ -1159,7 +1159,7 @@
         <v>45</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>88</v>
+        <v>175</v>
       </c>
       <c r="F4" s="4">
         <v>4</v>
@@ -1193,7 +1193,7 @@
         <v>45</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F5" s="4">
         <v>4</v>
@@ -1265,7 +1265,7 @@
         <v>45</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F7" s="7">
         <v>3</v>
@@ -1306,7 +1306,7 @@
         <v>45</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F8" s="4">
         <v>4</v>
@@ -1340,7 +1340,7 @@
         <v>45</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F9" s="4">
         <v>3</v>
@@ -1412,7 +1412,7 @@
         <v>45</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F11" s="7">
         <v>4</v>
@@ -1453,7 +1453,7 @@
         <v>45</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F12" s="4">
         <v>2</v>
@@ -1487,7 +1487,7 @@
         <v>45</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F13" s="4">
         <v>2</v>
@@ -1521,7 +1521,7 @@
         <v>45</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F14" s="4">
         <v>2</v>
@@ -1593,7 +1593,7 @@
         <v>45</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F16" s="4">
         <v>4</v>
@@ -1626,29 +1626,29 @@
       <c r="D17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="F17" s="4">
+      <c r="E17" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F17" s="7">
         <v>2</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="7">
         <v>450</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="7">
         <v>750</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="L17" s="4" t="s">
-        <v>172</v>
+      <c r="L17" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="N17" t="s">
         <v>60</v>
@@ -1668,7 +1668,7 @@
         <v>45</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F18" s="4">
         <v>3</v>
@@ -1702,7 +1702,7 @@
         <v>45</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>95</v>
+        <v>173</v>
       </c>
       <c r="F19" s="4">
         <v>3</v>
@@ -1710,8 +1710,12 @@
       <c r="G19" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="H19" s="4">
+        <v>1300</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1450</v>
+      </c>
       <c r="J19" s="4" t="s">
         <v>57</v>
       </c>
@@ -1719,7 +1723,7 @@
         <v>64</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>83</v>
+        <v>174</v>
       </c>
       <c r="N19" t="s">
         <v>53</v>
@@ -1739,7 +1743,7 @@
         <v>45</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F20" s="4">
         <v>3</v>
@@ -1811,7 +1815,7 @@
         <v>47</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>85</v>
+        <v>176</v>
       </c>
       <c r="F22" s="4">
         <v>4</v>
@@ -1828,7 +1832,7 @@
         <v>64</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -1883,7 +1887,7 @@
         <v>50</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F24" s="4">
         <v>2</v>
@@ -1900,7 +1904,7 @@
         <v>64</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -1917,7 +1921,7 @@
         <v>48</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F25" s="4">
         <v>2</v>
@@ -1948,7 +1952,7 @@
         <v>12</v>
       </c>
       <c r="J27" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K27">
         <f>COUNTIF(F2:F25, "=2")</f>
@@ -1964,7 +1968,7 @@
         <v>9</v>
       </c>
       <c r="J28" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K28">
         <f>COUNTIF(F2:F25, "=3")</f>
@@ -1982,7 +1986,7 @@
         <v>3</v>
       </c>
       <c r="J29" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K29">
         <f>COUNTIF(F2:F25, "=4")</f>
@@ -1991,7 +1995,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F30">
         <f>COUNTIF(J:J, "*DEF*")</f>
@@ -2060,16 +2064,16 @@
         <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -2086,17 +2090,17 @@
         <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2113,16 +2117,16 @@
         <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2139,17 +2143,17 @@
         <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2166,17 +2170,17 @@
         <v>45</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2193,17 +2197,17 @@
         <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2220,14 +2224,14 @@
         <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2244,16 +2248,16 @@
         <v>45</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" t="s">
         <v>127</v>
       </c>
-      <c r="F8" t="s">
-        <v>131</v>
-      </c>
       <c r="H8" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -2270,16 +2274,16 @@
         <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -2296,16 +2300,16 @@
         <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -2322,13 +2326,13 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -2345,16 +2349,16 @@
         <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2371,13 +2375,13 @@
         <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2394,13 +2398,13 @@
         <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2417,16 +2421,16 @@
         <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -2443,17 +2447,17 @@
         <v>45</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F16" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -2470,16 +2474,16 @@
         <v>45</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -2496,16 +2500,16 @@
         <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -2522,17 +2526,17 @@
         <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F19" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2549,16 +2553,16 @@
         <v>45</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -2575,16 +2579,16 @@
         <v>45</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="M21" s="1"/>
     </row>
@@ -2602,7 +2606,7 @@
         <v>47</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -2619,7 +2623,7 @@
         <v>49</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -2639,7 +2643,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -2656,7 +2660,7 @@
         <v>48</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Design and art for Legendary Samurai of the Wasteland is done, so now the Warrior slot is filled for the typal searchers.
</commit_message>
<xml_diff>
--- a/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
+++ b/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Format - 2005-08 Goat\Typal Battle Searchers\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2779EE6-BC4A-4FAE-8E94-7CAF4A7BA091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044AB07A-EE4D-461C-B35B-71544CBBCFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Single-Type Searchers" sheetId="1" r:id="rId1"/>
@@ -1017,7 +1017,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1701,28 +1701,28 @@
       <c r="D19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="7">
         <v>3</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="7">
         <v>1300</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="7">
         <v>1450</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="7" t="s">
         <v>174</v>
       </c>
       <c r="N19" t="s">

</xml_diff>

<commit_message>
Finished off Grassland Warrior and Vengeful Arbor, my Beast-Warrior and Plant searchers.
</commit_message>
<xml_diff>
--- a/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
+++ b/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Format - 2005-08 Goat\Typal Battle Searchers\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044AB07A-EE4D-461C-B35B-71544CBBCFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B55559-3690-4C38-91A3-521F3E720D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Single-Type Searchers" sheetId="1" r:id="rId1"/>
@@ -289,9 +289,6 @@
     <t>Horned Dolphin</t>
   </si>
   <si>
-    <t>Ancient Summoning Tree</t>
-  </si>
-  <si>
     <t>Infernal Gaze</t>
   </si>
   <si>
@@ -553,10 +550,13 @@
     <t>Zanki</t>
   </si>
   <si>
-    <t>Mountain Sentry</t>
-  </si>
-  <si>
     <t>Psychic Fiend</t>
+  </si>
+  <si>
+    <t>Grassland Warrior</t>
+  </si>
+  <si>
+    <t>Vengeful Arbor</t>
   </si>
 </sst>
 </file>
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1125,7 +1125,7 @@
         <v>45</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" s="4">
         <v>2</v>
@@ -1136,7 +1136,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>64</v>
@@ -1158,24 +1158,28 @@
       <c r="D4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="7">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
+      <c r="H4" s="7">
+        <v>900</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1500</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="7" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1193,7 +1197,7 @@
         <v>45</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F5" s="4">
         <v>4</v>
@@ -1265,7 +1269,7 @@
         <v>45</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F7" s="7">
         <v>3</v>
@@ -1306,7 +1310,7 @@
         <v>45</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F8" s="4">
         <v>4</v>
@@ -1412,7 +1416,7 @@
         <v>45</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F11" s="7">
         <v>4</v>
@@ -1452,24 +1456,28 @@
       <c r="D12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F12" s="4">
+      <c r="E12" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" s="7">
         <v>2</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4" t="s">
+      <c r="H12" s="7">
+        <v>800</v>
+      </c>
+      <c r="I12" s="7">
+        <v>1200</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="7" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1487,7 +1495,7 @@
         <v>45</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F13" s="4">
         <v>2</v>
@@ -1498,7 +1506,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>64</v>
@@ -1521,7 +1529,7 @@
         <v>45</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F14" s="4">
         <v>2</v>
@@ -1593,7 +1601,7 @@
         <v>45</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F16" s="4">
         <v>4</v>
@@ -1627,7 +1635,7 @@
         <v>45</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F17" s="7">
         <v>2</v>
@@ -1648,7 +1656,7 @@
         <v>64</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N17" t="s">
         <v>60</v>
@@ -1668,7 +1676,7 @@
         <v>45</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F18" s="4">
         <v>3</v>
@@ -1702,7 +1710,7 @@
         <v>45</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F19" s="7">
         <v>3</v>
@@ -1723,7 +1731,7 @@
         <v>64</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N19" t="s">
         <v>53</v>
@@ -1743,7 +1751,7 @@
         <v>45</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F20" s="4">
         <v>3</v>
@@ -1815,7 +1823,7 @@
         <v>47</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F22" s="4">
         <v>4</v>
@@ -1887,7 +1895,7 @@
         <v>50</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F24" s="4">
         <v>2</v>
@@ -1904,7 +1912,7 @@
         <v>64</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -1952,7 +1960,7 @@
         <v>12</v>
       </c>
       <c r="J27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K27">
         <f>COUNTIF(F2:F25, "=2")</f>
@@ -1968,7 +1976,7 @@
         <v>9</v>
       </c>
       <c r="J28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K28">
         <f>COUNTIF(F2:F25, "=3")</f>
@@ -1986,7 +1994,7 @@
         <v>3</v>
       </c>
       <c r="J29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K29">
         <f>COUNTIF(F2:F25, "=4")</f>
@@ -1995,7 +2003,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F30">
         <f>COUNTIF(J:J, "*DEF*")</f>
@@ -2064,16 +2072,16 @@
         <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -2090,17 +2098,17 @@
         <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2117,16 +2125,16 @@
         <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2143,17 +2151,17 @@
         <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2170,17 +2178,17 @@
         <v>45</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2197,17 +2205,17 @@
         <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2224,14 +2232,14 @@
         <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2248,16 +2256,16 @@
         <v>45</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -2274,16 +2282,16 @@
         <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -2300,16 +2308,16 @@
         <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H10" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -2326,13 +2334,13 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -2349,16 +2357,16 @@
         <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2375,13 +2383,13 @@
         <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2398,13 +2406,13 @@
         <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H14" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2421,16 +2429,16 @@
         <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -2447,17 +2455,17 @@
         <v>45</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -2474,16 +2482,16 @@
         <v>45</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -2500,16 +2508,16 @@
         <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -2526,17 +2534,17 @@
         <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2553,16 +2561,16 @@
         <v>45</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -2579,16 +2587,16 @@
         <v>45</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M21" s="1"/>
     </row>
@@ -2606,7 +2614,7 @@
         <v>47</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -2623,7 +2631,7 @@
         <v>49</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -2643,7 +2651,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -2660,7 +2668,7 @@
         <v>48</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shuffling set numbers around between Lava Eye, Lycanthrope, Synthesised, and Synthesis Fusion Ritual.
</commit_message>
<xml_diff>
--- a/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
+++ b/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Format - 2005-08 Goat\Typal Battle Searchers\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B55559-3690-4C38-91A3-521F3E720D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35171356-DCB6-4856-A1B9-E4893028F952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Single-Type Searchers" sheetId="1" r:id="rId1"/>
@@ -289,9 +289,6 @@
     <t>Horned Dolphin</t>
   </si>
   <si>
-    <t>Infernal Gaze</t>
-  </si>
-  <si>
     <t>Chameleon</t>
   </si>
   <si>
@@ -557,6 +554,9 @@
   </si>
   <si>
     <t>Vengeful Arbor</t>
+  </si>
+  <si>
+    <t>Lava Eye</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1017,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:L12"/>
+      <selection activeCell="E13" sqref="E13:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1125,7 +1125,7 @@
         <v>45</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" s="4">
         <v>2</v>
@@ -1159,7 +1159,7 @@
         <v>45</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F4" s="7">
         <v>4</v>
@@ -1197,7 +1197,7 @@
         <v>45</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F5" s="4">
         <v>4</v>
@@ -1269,7 +1269,7 @@
         <v>45</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F7" s="7">
         <v>3</v>
@@ -1310,7 +1310,7 @@
         <v>45</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F8" s="4">
         <v>4</v>
@@ -1416,7 +1416,7 @@
         <v>45</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F11" s="7">
         <v>4</v>
@@ -1457,7 +1457,7 @@
         <v>45</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F12" s="7">
         <v>2</v>
@@ -1494,24 +1494,28 @@
       <c r="D13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="4">
+      <c r="E13" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13" s="7">
         <v>2</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4" t="s">
+      <c r="H13" s="7">
+        <v>400</v>
+      </c>
+      <c r="I13" s="7">
+        <v>200</v>
+      </c>
+      <c r="J13" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="7" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1529,7 +1533,7 @@
         <v>45</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F14" s="4">
         <v>2</v>
@@ -1601,7 +1605,7 @@
         <v>45</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F16" s="4">
         <v>4</v>
@@ -1635,7 +1639,7 @@
         <v>45</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F17" s="7">
         <v>2</v>
@@ -1656,7 +1660,7 @@
         <v>64</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N17" t="s">
         <v>60</v>
@@ -1676,7 +1680,7 @@
         <v>45</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F18" s="4">
         <v>3</v>
@@ -1710,7 +1714,7 @@
         <v>45</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F19" s="7">
         <v>3</v>
@@ -1731,7 +1735,7 @@
         <v>64</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N19" t="s">
         <v>53</v>
@@ -1751,7 +1755,7 @@
         <v>45</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F20" s="4">
         <v>3</v>
@@ -1823,7 +1827,7 @@
         <v>47</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F22" s="4">
         <v>4</v>
@@ -1895,7 +1899,7 @@
         <v>50</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F24" s="4">
         <v>2</v>
@@ -1912,7 +1916,7 @@
         <v>64</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -1960,7 +1964,7 @@
         <v>12</v>
       </c>
       <c r="J27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K27">
         <f>COUNTIF(F2:F25, "=2")</f>
@@ -1976,7 +1980,7 @@
         <v>9</v>
       </c>
       <c r="J28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K28">
         <f>COUNTIF(F2:F25, "=3")</f>
@@ -1994,7 +1998,7 @@
         <v>3</v>
       </c>
       <c r="J29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K29">
         <f>COUNTIF(F2:F25, "=4")</f>
@@ -2003,7 +2007,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F30">
         <f>COUNTIF(J:J, "*DEF*")</f>
@@ -2072,16 +2076,16 @@
         <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -2098,17 +2102,17 @@
         <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2125,16 +2129,16 @@
         <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2151,17 +2155,17 @@
         <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2178,17 +2182,17 @@
         <v>45</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2205,17 +2209,17 @@
         <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2232,14 +2236,14 @@
         <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2256,16 +2260,16 @@
         <v>45</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -2282,16 +2286,16 @@
         <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -2308,16 +2312,16 @@
         <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H10" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -2334,13 +2338,13 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -2357,16 +2361,16 @@
         <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2383,13 +2387,13 @@
         <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2406,13 +2410,13 @@
         <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H14" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>141</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2429,16 +2433,16 @@
         <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -2455,17 +2459,17 @@
         <v>45</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -2482,16 +2486,16 @@
         <v>45</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -2508,16 +2512,16 @@
         <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -2534,17 +2538,17 @@
         <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2561,16 +2565,16 @@
         <v>45</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -2587,16 +2591,16 @@
         <v>45</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M21" s="1"/>
     </row>
@@ -2614,7 +2618,7 @@
         <v>47</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -2631,7 +2635,7 @@
         <v>49</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -2651,7 +2655,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -2668,7 +2672,7 @@
         <v>48</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished the Reptile typal battle searcher.
</commit_message>
<xml_diff>
--- a/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
+++ b/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Format - 2005-08 Goat\Typal Battle Searchers\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35171356-DCB6-4856-A1B9-E4893028F952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE93565E-1A03-46CF-B071-360D99EAE1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Single-Type Searchers" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="177">
   <si>
     <t>Attribute</t>
   </si>
@@ -622,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -632,6 +632,7 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1014,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1025,13 +1026,13 @@
     <col min="1" max="1" width="29.88671875" customWidth="1"/>
     <col min="2" max="2" width="4.109375" customWidth="1"/>
     <col min="3" max="3" width="3.44140625" customWidth="1"/>
-    <col min="4" max="4" width="5.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.77734375" customWidth="1"/>
+    <col min="7" max="7" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" customWidth="1"/>
-    <col min="11" max="11" width="9.77734375" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.77734375" customWidth="1"/>
   </cols>
@@ -1203,12 +1204,12 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>64</v>
@@ -1539,12 +1540,16 @@
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="H14" s="4">
+        <v>600</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
       <c r="J14" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>64</v>
@@ -1905,7 +1910,7 @@
         <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -1954,69 +1959,114 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27">
+        <f>COUNTIF(J:J, "*&lt;= 1500 ATK*")</f>
+        <v>14</v>
+      </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27">
-        <f>COUNTIF(J:J, "*&lt;= 1500 ATK*")</f>
-        <v>12</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="D27" t="s">
         <v>167</v>
       </c>
-      <c r="K27">
+      <c r="E27">
         <f>COUNTIF(F2:F25, "=2")</f>
         <v>8</v>
       </c>
+      <c r="G27" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27">
+        <f>COUNTIF(G2:G25, G27)</f>
+        <v>7</v>
+      </c>
+      <c r="J27" s="9"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E28" t="s">
+      <c r="A28" t="s">
         <v>59</v>
       </c>
-      <c r="F28">
+      <c r="B28">
         <f>COUNTIF(J:J, "*&lt;= 1500 DEF")</f>
-        <v>9</v>
-      </c>
-      <c r="J28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
         <v>168</v>
       </c>
-      <c r="K28">
+      <c r="E28">
         <f>COUNTIF(F2:F25, "=3")</f>
         <v>8</v>
       </c>
+      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28">
+        <f>COUNTIF(G2:G25, G28)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" t="s">
+      <c r="A29" t="s">
         <v>58</v>
       </c>
-      <c r="F29">
+      <c r="B29">
         <f>COUNTIF(J:J, "*&lt;= 2000 DEF*")</f>
         <v>3</v>
       </c>
-      <c r="J29" t="s">
+      <c r="C29" s="1"/>
+      <c r="D29" t="s">
         <v>169</v>
       </c>
-      <c r="K29">
+      <c r="E29">
         <f>COUNTIF(F2:F25, "=4")</f>
         <v>8</v>
       </c>
+      <c r="G29" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29">
+        <f>COUNTIF(G2:G25, G29)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E30" t="s">
+      <c r="A30" t="s">
         <v>96</v>
       </c>
-      <c r="F30">
+      <c r="B30">
         <f>COUNTIF(J:J, "*DEF*")</f>
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30">
+        <f>COUNTIF(G2:G25, G30)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31">
+        <f>COUNTIF(G2:G25, G31)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G32" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32">
+        <f>COUNTIF(G2:G25, G32)</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="G1:G26 G28:G1048576 E29:E30">
+  <conditionalFormatting sqref="A29:A30 G1:G1048576">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"DARK"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Finished this week's typal battle searcher. For Beast monsters: Armordillo Rat.
</commit_message>
<xml_diff>
--- a/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
+++ b/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Format - 2005-08 Goat\Typal Battle Searchers\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE93565E-1A03-46CF-B071-360D99EAE1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D842F178-804F-4D83-B323-7FE638795756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -622,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -632,7 +632,6 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1017,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1134,8 +1133,12 @@
       <c r="G3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="H3" s="4">
+        <v>450</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1200</v>
+      </c>
       <c r="J3" s="4" t="s">
         <v>59</v>
       </c>
@@ -1533,28 +1536,28 @@
       <c r="D14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="7">
         <v>2</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="7">
         <v>600</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="7">
         <v>0</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="7" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1981,7 +1984,6 @@
         <f>COUNTIF(G2:G25, G27)</f>
         <v>7</v>
       </c>
-      <c r="J27" s="9"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -2066,7 +2068,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A29:A30 G1:G1048576">
+  <conditionalFormatting sqref="G1:G1048576 A29:A30">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"DARK"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated the typal searcher collages.
</commit_message>
<xml_diff>
--- a/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
+++ b/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Format - 2005-08 Goat\Typal Battle Searchers\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D842F178-804F-4D83-B323-7FE638795756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016D4E22-0C61-45BB-B66B-5150293E2971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Single-Type Searchers" sheetId="1" r:id="rId1"/>
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,28 +1124,28 @@
       <c r="D3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="7">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="7">
         <v>450</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="7">
         <v>1200</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="7" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1621,8 +1621,12 @@
       <c r="G16" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="H16" s="4">
+        <v>1400</v>
+      </c>
+      <c r="I16" s="4">
+        <v>1200</v>
+      </c>
       <c r="J16" s="4" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
Minor change to Typal Searchers spreadsheet that I forget what it was, would have happened while I was making those notes for an elemental Fusion archetype.
</commit_message>
<xml_diff>
--- a/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
+++ b/Custom Cards/Format - 2005-08 Goat/Typal Battle Searchers/Designs/Typal Searchers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Format - 2005-08 Goat\Typal Battle Searchers\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016D4E22-0C61-45BB-B66B-5150293E2971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37F0B67-8959-4BF2-8754-4BBB5753221A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Single-Type Searchers" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="177">
   <si>
     <t>Attribute</t>
   </si>
@@ -563,7 +563,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -577,8 +577,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -609,6 +616,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -622,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -632,6 +663,10 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1033,7 +1068,7 @@
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.77734375" customWidth="1"/>
+    <col min="13" max="13" width="6.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -1073,6 +1108,9 @@
       <c r="L1" t="s">
         <v>65</v>
       </c>
+      <c r="M1" t="s">
+        <v>97</v>
+      </c>
       <c r="N1" t="s">
         <v>52</v>
       </c>
@@ -1110,6 +1148,9 @@
       <c r="L2" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="M2" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1220,6 +1261,9 @@
       <c r="L5" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="M5" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1333,6 +1377,9 @@
       <c r="L8" s="4" t="s">
         <v>72</v>
       </c>
+      <c r="M8" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1367,6 +1414,9 @@
       <c r="L9" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="M9" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1635,6 +1685,9 @@
       </c>
       <c r="L16" s="4" t="s">
         <v>82</v>
+      </c>
+      <c r="M16" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1711,6 +1764,9 @@
       <c r="L18" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="M18" s="11">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -1786,6 +1842,9 @@
       <c r="L20" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="M20" s="11">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -1858,6 +1917,9 @@
       <c r="L22" s="4" t="s">
         <v>83</v>
       </c>
+      <c r="M22" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -1930,6 +1992,9 @@
       <c r="L24" s="4" t="s">
         <v>91</v>
       </c>
+      <c r="M24" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -1963,6 +2028,9 @@
       </c>
       <c r="L25" s="4" t="s">
         <v>80</v>
+      </c>
+      <c r="M25" s="12">
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>